<commit_message>
v3 Ok ça rend PAS MAL hein
</commit_message>
<xml_diff>
--- a/output/OccilanStats.xlsx
+++ b/output/OccilanStats.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tournoi" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Records" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Bots Intermédiaires" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Burger Frites" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="EC Emerald" sheetId="4" state="visible" r:id="rId4"/>
@@ -75,15 +75,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -466,7 +469,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Statistiques globales du tournoi</t>
+          <t>Records du tournoi</t>
         </is>
       </c>
     </row>
@@ -495,121 +498,201 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>Total kills</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="n"/>
-      <c r="C3" s="3" t="n"/>
+          <t>Plus grand nombre de kills</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>Thibee</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>La Ruche</t>
+        </is>
+      </c>
       <c r="D3" s="3" t="n">
-        <v/>
+        <v>152</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>Total deaths</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="n"/>
-      <c r="C4" s="3" t="n"/>
+          <t>Plus grand nombre de morts</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Colfeo</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>La Ruche</t>
+        </is>
+      </c>
       <c r="D4" s="3" t="n">
-        <v/>
+        <v>76</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>Total assists</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="n"/>
-      <c r="C5" s="3" t="n"/>
+          <t>Plus grand nombre d'assists</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Xintox</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>La Ruche</t>
+        </is>
+      </c>
       <c r="D5" s="3" t="n">
-        <v/>
+        <v>282</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>Average kills</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="n"/>
-      <c r="C6" s="3" t="n"/>
+          <t>Meilleure moyenne de kills</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>KCDQ Bangala</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>KCDQ</t>
+        </is>
+      </c>
       <c r="D6" s="3" t="n">
-        <v/>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>Average deaths</t>
-        </is>
-      </c>
-      <c r="B7" s="3" t="n"/>
-      <c r="C7" s="3" t="n"/>
+          <t>Plus faible moyenne de morts</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>manchou</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>La bande du PMU</t>
+        </is>
+      </c>
       <c r="D7" s="3" t="n">
-        <v/>
+        <v>6.7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>Average assists</t>
-        </is>
-      </c>
-      <c r="B8" s="3" t="n"/>
-      <c r="C8" s="3" t="n"/>
+          <t>Meilleure moyenne d'assists</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>Xintox</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>La Ruche</t>
+        </is>
+      </c>
       <c r="D8" s="3" t="n">
-        <v/>
+        <v>14.1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>Average kda</t>
-        </is>
-      </c>
-      <c r="B9" s="3" t="n"/>
-      <c r="C9" s="3" t="n"/>
+          <t>Meilleur KDA</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>climber</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>La Ruche</t>
+        </is>
+      </c>
       <c r="D9" s="3" t="n">
-        <v/>
+        <v>6.2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>Average cs per minute</t>
-        </is>
-      </c>
-      <c r="B10" s="3" t="n"/>
-      <c r="C10" s="3" t="n"/>
+          <t>Meilleur CS/min</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>Thibee</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>La Ruche</t>
+        </is>
+      </c>
       <c r="D10" s="3" t="n">
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>Unique champions played</t>
-        </is>
-      </c>
-      <c r="B11" s="3" t="n"/>
-      <c r="C11" s="3" t="n"/>
+          <t>Meilleur score de vision</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>Bob Le Tripoteur</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>Gungnir</t>
+        </is>
+      </c>
       <c r="D11" s="3" t="n">
-        <v/>
+        <v>103</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>Average vision score</t>
-        </is>
-      </c>
-      <c r="B12" s="3" t="n"/>
-      <c r="C12" s="3" t="n"/>
+          <t>Plus de champions joués</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>Thibee</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>La Ruche</t>
+        </is>
+      </c>
       <c r="D12" s="3" t="n">
-        <v/>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -626,7 +709,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -634,29 +717,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="40" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Statistiques globales de l'équipe La Sauce Du Chef</t>
+          <t>Statistiques de La Sauce Du Chef</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nombre de parties jouées</t>
+          <t>Matchs joués</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -666,7 +747,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nombre de victoires</t>
+          <t>Victoires</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -676,7 +757,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nombre de défaites</t>
+          <t>Défaites</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -698,7 +779,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Durée moyenne des parties</t>
+          <t>Durée moyenne</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -710,7 +791,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Partie la plus rapide</t>
+          <t>Plus court</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -722,7 +803,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Partie la plus longue</t>
+          <t>Plus long</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -732,9 +813,9 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Statistiques par joueur</t>
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Statistiques des joueurs</t>
         </is>
       </c>
     </row>
@@ -751,32 +832,32 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Kills moy.</t>
+          <t>Kills/G</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>Deaths moy.</t>
+          <t>Deaths/G</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Assists moy.</t>
+          <t>Assists/G</t>
         </is>
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>CS/M moy.</t>
+          <t>CS/min</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Vision moy.</t>
+          <t>Vision/G</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>Champions joués</t>
+          <t>Champions</t>
         </is>
       </c>
     </row>
@@ -870,68 +951,9 @@
         </is>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>Détail des parties</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="inlineStr">
-        <is>
-          <t>Match ID</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="inlineStr">
-        <is>
-          <t>Joueur</t>
-        </is>
-      </c>
-      <c r="C20" s="2" t="inlineStr">
-        <is>
-          <t>Champion</t>
-        </is>
-      </c>
-      <c r="D20" s="2" t="inlineStr">
-        <is>
-          <t>KDA</t>
-        </is>
-      </c>
-      <c r="E20" s="2" t="inlineStr">
-        <is>
-          <t>K/D/A</t>
-        </is>
-      </c>
-      <c r="F20" s="2" t="inlineStr">
-        <is>
-          <t>CS</t>
-        </is>
-      </c>
-      <c r="G20" s="2" t="inlineStr">
-        <is>
-          <t>CS/min</t>
-        </is>
-      </c>
-      <c r="H20" s="2" t="inlineStr">
-        <is>
-          <t>Vision Score</t>
-        </is>
-      </c>
-      <c r="I20" s="2" t="inlineStr">
-        <is>
-          <t>Résultat</t>
-        </is>
-      </c>
-      <c r="J20" s="2" t="inlineStr">
-        <is>
-          <t>Durée</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -943,7 +965,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -951,29 +973,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="40" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Statistiques globales de l'équipe Les minorités</t>
+          <t>Statistiques de Les minorités</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nombre de parties jouées</t>
+          <t>Matchs joués</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -983,7 +1003,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nombre de victoires</t>
+          <t>Victoires</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -993,7 +1013,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nombre de défaites</t>
+          <t>Défaites</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1015,7 +1035,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Durée moyenne des parties</t>
+          <t>Durée moyenne</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1027,7 +1047,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Partie la plus rapide</t>
+          <t>Plus court</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1039,7 +1059,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Partie la plus longue</t>
+          <t>Plus long</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1049,9 +1069,9 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Statistiques par joueur</t>
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Statistiques des joueurs</t>
         </is>
       </c>
     </row>
@@ -1068,32 +1088,32 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Kills moy.</t>
+          <t>Kills/G</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>Deaths moy.</t>
+          <t>Deaths/G</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Assists moy.</t>
+          <t>Assists/G</t>
         </is>
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>CS/M moy.</t>
+          <t>CS/min</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Vision moy.</t>
+          <t>Vision/G</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>Champions joués</t>
+          <t>Champions</t>
         </is>
       </c>
     </row>
@@ -1247,68 +1267,9 @@
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Détail des parties</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>Match ID</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>Joueur</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>Champion</t>
-        </is>
-      </c>
-      <c r="D22" s="2" t="inlineStr">
-        <is>
-          <t>KDA</t>
-        </is>
-      </c>
-      <c r="E22" s="2" t="inlineStr">
-        <is>
-          <t>K/D/A</t>
-        </is>
-      </c>
-      <c r="F22" s="2" t="inlineStr">
-        <is>
-          <t>CS</t>
-        </is>
-      </c>
-      <c r="G22" s="2" t="inlineStr">
-        <is>
-          <t>CS/min</t>
-        </is>
-      </c>
-      <c r="H22" s="2" t="inlineStr">
-        <is>
-          <t>Vision Score</t>
-        </is>
-      </c>
-      <c r="I22" s="2" t="inlineStr">
-        <is>
-          <t>Résultat</t>
-        </is>
-      </c>
-      <c r="J22" s="2" t="inlineStr">
-        <is>
-          <t>Durée</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1320,7 +1281,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1328,29 +1289,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="40" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Statistiques globales de l'équipe LIONS GUARD</t>
+          <t>Statistiques de LIONS GUARD</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nombre de parties jouées</t>
+          <t>Matchs joués</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1360,7 +1319,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nombre de victoires</t>
+          <t>Victoires</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1370,7 +1329,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nombre de défaites</t>
+          <t>Défaites</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1392,7 +1351,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Durée moyenne des parties</t>
+          <t>Durée moyenne</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1404,7 +1363,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Partie la plus rapide</t>
+          <t>Plus court</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1416,7 +1375,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Partie la plus longue</t>
+          <t>Plus long</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1426,9 +1385,9 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Statistiques par joueur</t>
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Statistiques des joueurs</t>
         </is>
       </c>
     </row>
@@ -1445,32 +1404,32 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Kills moy.</t>
+          <t>Kills/G</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>Deaths moy.</t>
+          <t>Deaths/G</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Assists moy.</t>
+          <t>Assists/G</t>
         </is>
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>CS/M moy.</t>
+          <t>CS/min</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Vision moy.</t>
+          <t>Vision/G</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>Champions joués</t>
+          <t>Champions</t>
         </is>
       </c>
     </row>
@@ -1624,68 +1583,9 @@
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Détail des parties</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>Match ID</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>Joueur</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>Champion</t>
-        </is>
-      </c>
-      <c r="D22" s="2" t="inlineStr">
-        <is>
-          <t>KDA</t>
-        </is>
-      </c>
-      <c r="E22" s="2" t="inlineStr">
-        <is>
-          <t>K/D/A</t>
-        </is>
-      </c>
-      <c r="F22" s="2" t="inlineStr">
-        <is>
-          <t>CS</t>
-        </is>
-      </c>
-      <c r="G22" s="2" t="inlineStr">
-        <is>
-          <t>CS/min</t>
-        </is>
-      </c>
-      <c r="H22" s="2" t="inlineStr">
-        <is>
-          <t>Vision Score</t>
-        </is>
-      </c>
-      <c r="I22" s="2" t="inlineStr">
-        <is>
-          <t>Résultat</t>
-        </is>
-      </c>
-      <c r="J22" s="2" t="inlineStr">
-        <is>
-          <t>Durée</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1697,7 +1597,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1705,29 +1605,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="40" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Statistiques globales de l'équipe Mickey Mouse Club</t>
+          <t>Statistiques de Mickey Mouse Club</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nombre de parties jouées</t>
+          <t>Matchs joués</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1737,7 +1635,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nombre de victoires</t>
+          <t>Victoires</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1747,7 +1645,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nombre de défaites</t>
+          <t>Défaites</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1769,7 +1667,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Durée moyenne des parties</t>
+          <t>Durée moyenne</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1781,7 +1679,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Partie la plus rapide</t>
+          <t>Plus court</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1793,7 +1691,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Partie la plus longue</t>
+          <t>Plus long</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1803,9 +1701,9 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Statistiques par joueur</t>
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Statistiques des joueurs</t>
         </is>
       </c>
     </row>
@@ -1822,32 +1720,32 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Kills moy.</t>
+          <t>Kills/G</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>Deaths moy.</t>
+          <t>Deaths/G</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Assists moy.</t>
+          <t>Assists/G</t>
         </is>
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>CS/M moy.</t>
+          <t>CS/min</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Vision moy.</t>
+          <t>Vision/G</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>Champions joués</t>
+          <t>Champions</t>
         </is>
       </c>
     </row>
@@ -2001,68 +1899,9 @@
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Détail des parties</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>Match ID</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>Joueur</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>Champion</t>
-        </is>
-      </c>
-      <c r="D22" s="2" t="inlineStr">
-        <is>
-          <t>KDA</t>
-        </is>
-      </c>
-      <c r="E22" s="2" t="inlineStr">
-        <is>
-          <t>K/D/A</t>
-        </is>
-      </c>
-      <c r="F22" s="2" t="inlineStr">
-        <is>
-          <t>CS</t>
-        </is>
-      </c>
-      <c r="G22" s="2" t="inlineStr">
-        <is>
-          <t>CS/min</t>
-        </is>
-      </c>
-      <c r="H22" s="2" t="inlineStr">
-        <is>
-          <t>Vision Score</t>
-        </is>
-      </c>
-      <c r="I22" s="2" t="inlineStr">
-        <is>
-          <t>Résultat</t>
-        </is>
-      </c>
-      <c r="J22" s="2" t="inlineStr">
-        <is>
-          <t>Durée</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2074,7 +1913,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2082,29 +1921,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="40" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Statistiques globales de l'équipe Pas de quartier</t>
+          <t>Statistiques de Pas de quartier</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nombre de parties jouées</t>
+          <t>Matchs joués</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2114,7 +1951,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nombre de victoires</t>
+          <t>Victoires</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2124,7 +1961,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nombre de défaites</t>
+          <t>Défaites</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2146,7 +1983,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Durée moyenne des parties</t>
+          <t>Durée moyenne</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2158,7 +1995,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Partie la plus rapide</t>
+          <t>Plus court</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2170,7 +2007,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Partie la plus longue</t>
+          <t>Plus long</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2180,9 +2017,9 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Statistiques par joueur</t>
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Statistiques des joueurs</t>
         </is>
       </c>
     </row>
@@ -2199,32 +2036,32 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Kills moy.</t>
+          <t>Kills/G</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>Deaths moy.</t>
+          <t>Deaths/G</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Assists moy.</t>
+          <t>Assists/G</t>
         </is>
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>CS/M moy.</t>
+          <t>CS/min</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Vision moy.</t>
+          <t>Vision/G</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>Champions joués</t>
+          <t>Champions</t>
         </is>
       </c>
     </row>
@@ -2378,68 +2215,9 @@
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Détail des parties</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>Match ID</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>Joueur</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>Champion</t>
-        </is>
-      </c>
-      <c r="D22" s="2" t="inlineStr">
-        <is>
-          <t>KDA</t>
-        </is>
-      </c>
-      <c r="E22" s="2" t="inlineStr">
-        <is>
-          <t>K/D/A</t>
-        </is>
-      </c>
-      <c r="F22" s="2" t="inlineStr">
-        <is>
-          <t>CS</t>
-        </is>
-      </c>
-      <c r="G22" s="2" t="inlineStr">
-        <is>
-          <t>CS/min</t>
-        </is>
-      </c>
-      <c r="H22" s="2" t="inlineStr">
-        <is>
-          <t>Vision Score</t>
-        </is>
-      </c>
-      <c r="I22" s="2" t="inlineStr">
-        <is>
-          <t>Résultat</t>
-        </is>
-      </c>
-      <c r="J22" s="2" t="inlineStr">
-        <is>
-          <t>Durée</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2451,7 +2229,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2459,29 +2237,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="40" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Statistiques globales de l'équipe PCS Genuise</t>
+          <t>Statistiques de PCS Genuise</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nombre de parties jouées</t>
+          <t>Matchs joués</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2491,7 +2267,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nombre de victoires</t>
+          <t>Victoires</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2501,7 +2277,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nombre de défaites</t>
+          <t>Défaites</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2523,7 +2299,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Durée moyenne des parties</t>
+          <t>Durée moyenne</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2535,7 +2311,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Partie la plus rapide</t>
+          <t>Plus court</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2547,7 +2323,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Partie la plus longue</t>
+          <t>Plus long</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2557,9 +2333,9 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Statistiques par joueur</t>
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Statistiques des joueurs</t>
         </is>
       </c>
     </row>
@@ -2576,32 +2352,32 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Kills moy.</t>
+          <t>Kills/G</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>Deaths moy.</t>
+          <t>Deaths/G</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Assists moy.</t>
+          <t>Assists/G</t>
         </is>
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>CS/M moy.</t>
+          <t>CS/min</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Vision moy.</t>
+          <t>Vision/G</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>Champions joués</t>
+          <t>Champions</t>
         </is>
       </c>
     </row>
@@ -2725,68 +2501,9 @@
         </is>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>Détail des parties</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="inlineStr">
-        <is>
-          <t>Match ID</t>
-        </is>
-      </c>
-      <c r="B21" s="2" t="inlineStr">
-        <is>
-          <t>Joueur</t>
-        </is>
-      </c>
-      <c r="C21" s="2" t="inlineStr">
-        <is>
-          <t>Champion</t>
-        </is>
-      </c>
-      <c r="D21" s="2" t="inlineStr">
-        <is>
-          <t>KDA</t>
-        </is>
-      </c>
-      <c r="E21" s="2" t="inlineStr">
-        <is>
-          <t>K/D/A</t>
-        </is>
-      </c>
-      <c r="F21" s="2" t="inlineStr">
-        <is>
-          <t>CS</t>
-        </is>
-      </c>
-      <c r="G21" s="2" t="inlineStr">
-        <is>
-          <t>CS/min</t>
-        </is>
-      </c>
-      <c r="H21" s="2" t="inlineStr">
-        <is>
-          <t>Vision Score</t>
-        </is>
-      </c>
-      <c r="I21" s="2" t="inlineStr">
-        <is>
-          <t>Résultat</t>
-        </is>
-      </c>
-      <c r="J21" s="2" t="inlineStr">
-        <is>
-          <t>Durée</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2798,7 +2515,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2806,29 +2523,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="40" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Statistiques globales de l'équipe Pipi Gaming</t>
+          <t>Statistiques de Pipi Gaming</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nombre de parties jouées</t>
+          <t>Matchs joués</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2838,7 +2553,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nombre de victoires</t>
+          <t>Victoires</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2848,7 +2563,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nombre de défaites</t>
+          <t>Défaites</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2870,7 +2585,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Durée moyenne des parties</t>
+          <t>Durée moyenne</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2882,7 +2597,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Partie la plus rapide</t>
+          <t>Plus court</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2894,7 +2609,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Partie la plus longue</t>
+          <t>Plus long</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2904,9 +2619,9 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Statistiques par joueur</t>
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Statistiques des joueurs</t>
         </is>
       </c>
     </row>
@@ -2923,32 +2638,32 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Kills moy.</t>
+          <t>Kills/G</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>Deaths moy.</t>
+          <t>Deaths/G</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Assists moy.</t>
+          <t>Assists/G</t>
         </is>
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>CS/M moy.</t>
+          <t>CS/min</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Vision moy.</t>
+          <t>Vision/G</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>Champions joués</t>
+          <t>Champions</t>
         </is>
       </c>
     </row>
@@ -3102,68 +2817,9 @@
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Détail des parties</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>Match ID</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>Joueur</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>Champion</t>
-        </is>
-      </c>
-      <c r="D22" s="2" t="inlineStr">
-        <is>
-          <t>KDA</t>
-        </is>
-      </c>
-      <c r="E22" s="2" t="inlineStr">
-        <is>
-          <t>K/D/A</t>
-        </is>
-      </c>
-      <c r="F22" s="2" t="inlineStr">
-        <is>
-          <t>CS</t>
-        </is>
-      </c>
-      <c r="G22" s="2" t="inlineStr">
-        <is>
-          <t>CS/min</t>
-        </is>
-      </c>
-      <c r="H22" s="2" t="inlineStr">
-        <is>
-          <t>Vision Score</t>
-        </is>
-      </c>
-      <c r="I22" s="2" t="inlineStr">
-        <is>
-          <t>Résultat</t>
-        </is>
-      </c>
-      <c r="J22" s="2" t="inlineStr">
-        <is>
-          <t>Durée</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -3175,7 +2831,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3183,29 +2839,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="40" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Statistiques globales de l'équipe zizicacacorp</t>
+          <t>Statistiques de zizicacacorp</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nombre de parties jouées</t>
+          <t>Matchs joués</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -3215,7 +2869,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nombre de victoires</t>
+          <t>Victoires</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -3225,7 +2879,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nombre de défaites</t>
+          <t>Défaites</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -3247,7 +2901,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Durée moyenne des parties</t>
+          <t>Durée moyenne</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -3259,7 +2913,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Partie la plus rapide</t>
+          <t>Plus court</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -3271,7 +2925,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Partie la plus longue</t>
+          <t>Plus long</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -3281,9 +2935,9 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Statistiques par joueur</t>
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Statistiques des joueurs</t>
         </is>
       </c>
     </row>
@@ -3300,32 +2954,32 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Kills moy.</t>
+          <t>Kills/G</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>Deaths moy.</t>
+          <t>Deaths/G</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Assists moy.</t>
+          <t>Assists/G</t>
         </is>
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>CS/M moy.</t>
+          <t>CS/min</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Vision moy.</t>
+          <t>Vision/G</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>Champions joués</t>
+          <t>Champions</t>
         </is>
       </c>
     </row>
@@ -3479,68 +3133,9 @@
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Détail des parties</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>Match ID</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>Joueur</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>Champion</t>
-        </is>
-      </c>
-      <c r="D22" s="2" t="inlineStr">
-        <is>
-          <t>KDA</t>
-        </is>
-      </c>
-      <c r="E22" s="2" t="inlineStr">
-        <is>
-          <t>K/D/A</t>
-        </is>
-      </c>
-      <c r="F22" s="2" t="inlineStr">
-        <is>
-          <t>CS</t>
-        </is>
-      </c>
-      <c r="G22" s="2" t="inlineStr">
-        <is>
-          <t>CS/min</t>
-        </is>
-      </c>
-      <c r="H22" s="2" t="inlineStr">
-        <is>
-          <t>Vision Score</t>
-        </is>
-      </c>
-      <c r="I22" s="2" t="inlineStr">
-        <is>
-          <t>Résultat</t>
-        </is>
-      </c>
-      <c r="J22" s="2" t="inlineStr">
-        <is>
-          <t>Durée</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -3552,7 +3147,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3560,29 +3155,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="40" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Statistiques globales de l'équipe Bots Intermédiaires</t>
+          <t>Statistiques de Bots Intermédiaires</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nombre de parties jouées</t>
+          <t>Matchs joués</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -3592,7 +3185,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nombre de victoires</t>
+          <t>Victoires</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -3602,7 +3195,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nombre de défaites</t>
+          <t>Défaites</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -3624,7 +3217,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Durée moyenne des parties</t>
+          <t>Durée moyenne</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -3636,7 +3229,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Partie la plus rapide</t>
+          <t>Plus court</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -3648,7 +3241,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Partie la plus longue</t>
+          <t>Plus long</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -3658,9 +3251,9 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Statistiques par joueur</t>
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Statistiques des joueurs</t>
         </is>
       </c>
     </row>
@@ -3677,32 +3270,32 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Kills moy.</t>
+          <t>Kills/G</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>Deaths moy.</t>
+          <t>Deaths/G</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Assists moy.</t>
+          <t>Assists/G</t>
         </is>
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>CS/M moy.</t>
+          <t>CS/min</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Vision moy.</t>
+          <t>Vision/G</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>Champions joués</t>
+          <t>Champions</t>
         </is>
       </c>
     </row>
@@ -3856,68 +3449,9 @@
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Détail des parties</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>Match ID</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>Joueur</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>Champion</t>
-        </is>
-      </c>
-      <c r="D22" s="2" t="inlineStr">
-        <is>
-          <t>KDA</t>
-        </is>
-      </c>
-      <c r="E22" s="2" t="inlineStr">
-        <is>
-          <t>K/D/A</t>
-        </is>
-      </c>
-      <c r="F22" s="2" t="inlineStr">
-        <is>
-          <t>CS</t>
-        </is>
-      </c>
-      <c r="G22" s="2" t="inlineStr">
-        <is>
-          <t>CS/min</t>
-        </is>
-      </c>
-      <c r="H22" s="2" t="inlineStr">
-        <is>
-          <t>Vision Score</t>
-        </is>
-      </c>
-      <c r="I22" s="2" t="inlineStr">
-        <is>
-          <t>Résultat</t>
-        </is>
-      </c>
-      <c r="J22" s="2" t="inlineStr">
-        <is>
-          <t>Durée</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -3929,7 +3463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3937,29 +3471,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="40" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Statistiques globales de l'équipe Burger Frites</t>
+          <t>Statistiques de Burger Frites</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nombre de parties jouées</t>
+          <t>Matchs joués</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -3969,7 +3501,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nombre de victoires</t>
+          <t>Victoires</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -3979,7 +3511,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nombre de défaites</t>
+          <t>Défaites</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -4001,7 +3533,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Durée moyenne des parties</t>
+          <t>Durée moyenne</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -4013,7 +3545,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Partie la plus rapide</t>
+          <t>Plus court</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -4025,7 +3557,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Partie la plus longue</t>
+          <t>Plus long</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -4035,9 +3567,9 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Statistiques par joueur</t>
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Statistiques des joueurs</t>
         </is>
       </c>
     </row>
@@ -4054,32 +3586,32 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Kills moy.</t>
+          <t>Kills/G</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>Deaths moy.</t>
+          <t>Deaths/G</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Assists moy.</t>
+          <t>Assists/G</t>
         </is>
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>CS/M moy.</t>
+          <t>CS/min</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Vision moy.</t>
+          <t>Vision/G</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>Champions joués</t>
+          <t>Champions</t>
         </is>
       </c>
     </row>
@@ -4203,68 +3735,9 @@
         </is>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>Détail des parties</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="inlineStr">
-        <is>
-          <t>Match ID</t>
-        </is>
-      </c>
-      <c r="B21" s="2" t="inlineStr">
-        <is>
-          <t>Joueur</t>
-        </is>
-      </c>
-      <c r="C21" s="2" t="inlineStr">
-        <is>
-          <t>Champion</t>
-        </is>
-      </c>
-      <c r="D21" s="2" t="inlineStr">
-        <is>
-          <t>KDA</t>
-        </is>
-      </c>
-      <c r="E21" s="2" t="inlineStr">
-        <is>
-          <t>K/D/A</t>
-        </is>
-      </c>
-      <c r="F21" s="2" t="inlineStr">
-        <is>
-          <t>CS</t>
-        </is>
-      </c>
-      <c r="G21" s="2" t="inlineStr">
-        <is>
-          <t>CS/min</t>
-        </is>
-      </c>
-      <c r="H21" s="2" t="inlineStr">
-        <is>
-          <t>Vision Score</t>
-        </is>
-      </c>
-      <c r="I21" s="2" t="inlineStr">
-        <is>
-          <t>Résultat</t>
-        </is>
-      </c>
-      <c r="J21" s="2" t="inlineStr">
-        <is>
-          <t>Durée</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4276,7 +3749,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4284,29 +3757,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="40" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Statistiques globales de l'équipe EC Emerald</t>
+          <t>Statistiques de EC Emerald</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nombre de parties jouées</t>
+          <t>Matchs joués</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -4316,7 +3787,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nombre de victoires</t>
+          <t>Victoires</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -4326,7 +3797,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nombre de défaites</t>
+          <t>Défaites</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -4348,7 +3819,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Durée moyenne des parties</t>
+          <t>Durée moyenne</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -4360,7 +3831,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Partie la plus rapide</t>
+          <t>Plus court</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -4372,7 +3843,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Partie la plus longue</t>
+          <t>Plus long</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -4382,9 +3853,9 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Statistiques par joueur</t>
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Statistiques des joueurs</t>
         </is>
       </c>
     </row>
@@ -4401,32 +3872,32 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Kills moy.</t>
+          <t>Kills/G</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>Deaths moy.</t>
+          <t>Deaths/G</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Assists moy.</t>
+          <t>Assists/G</t>
         </is>
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>CS/M moy.</t>
+          <t>CS/min</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Vision moy.</t>
+          <t>Vision/G</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>Champions joués</t>
+          <t>Champions</t>
         </is>
       </c>
     </row>
@@ -4580,68 +4051,9 @@
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Détail des parties</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>Match ID</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>Joueur</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>Champion</t>
-        </is>
-      </c>
-      <c r="D22" s="2" t="inlineStr">
-        <is>
-          <t>KDA</t>
-        </is>
-      </c>
-      <c r="E22" s="2" t="inlineStr">
-        <is>
-          <t>K/D/A</t>
-        </is>
-      </c>
-      <c r="F22" s="2" t="inlineStr">
-        <is>
-          <t>CS</t>
-        </is>
-      </c>
-      <c r="G22" s="2" t="inlineStr">
-        <is>
-          <t>CS/min</t>
-        </is>
-      </c>
-      <c r="H22" s="2" t="inlineStr">
-        <is>
-          <t>Vision Score</t>
-        </is>
-      </c>
-      <c r="I22" s="2" t="inlineStr">
-        <is>
-          <t>Résultat</t>
-        </is>
-      </c>
-      <c r="J22" s="2" t="inlineStr">
-        <is>
-          <t>Durée</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4653,7 +4065,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4661,29 +4073,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="40" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Statistiques globales de l'équipe GIRL POWDER</t>
+          <t>Statistiques de GIRL POWDER</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nombre de parties jouées</t>
+          <t>Matchs joués</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -4693,7 +4103,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nombre de victoires</t>
+          <t>Victoires</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -4703,7 +4113,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nombre de défaites</t>
+          <t>Défaites</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -4725,7 +4135,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Durée moyenne des parties</t>
+          <t>Durée moyenne</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -4737,7 +4147,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Partie la plus rapide</t>
+          <t>Plus court</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -4749,7 +4159,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Partie la plus longue</t>
+          <t>Plus long</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -4759,9 +4169,9 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Statistiques par joueur</t>
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Statistiques des joueurs</t>
         </is>
       </c>
     </row>
@@ -4778,32 +4188,32 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Kills moy.</t>
+          <t>Kills/G</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>Deaths moy.</t>
+          <t>Deaths/G</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Assists moy.</t>
+          <t>Assists/G</t>
         </is>
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>CS/M moy.</t>
+          <t>CS/min</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Vision moy.</t>
+          <t>Vision/G</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>Champions joués</t>
+          <t>Champions</t>
         </is>
       </c>
     </row>
@@ -4957,68 +4367,9 @@
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Détail des parties</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>Match ID</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>Joueur</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>Champion</t>
-        </is>
-      </c>
-      <c r="D22" s="2" t="inlineStr">
-        <is>
-          <t>KDA</t>
-        </is>
-      </c>
-      <c r="E22" s="2" t="inlineStr">
-        <is>
-          <t>K/D/A</t>
-        </is>
-      </c>
-      <c r="F22" s="2" t="inlineStr">
-        <is>
-          <t>CS</t>
-        </is>
-      </c>
-      <c r="G22" s="2" t="inlineStr">
-        <is>
-          <t>CS/min</t>
-        </is>
-      </c>
-      <c r="H22" s="2" t="inlineStr">
-        <is>
-          <t>Vision Score</t>
-        </is>
-      </c>
-      <c r="I22" s="2" t="inlineStr">
-        <is>
-          <t>Résultat</t>
-        </is>
-      </c>
-      <c r="J22" s="2" t="inlineStr">
-        <is>
-          <t>Durée</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5030,7 +4381,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5038,29 +4389,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="40" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Statistiques globales de l'équipe Gungnir</t>
+          <t>Statistiques de Gungnir</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nombre de parties jouées</t>
+          <t>Matchs joués</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -5070,7 +4419,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nombre de victoires</t>
+          <t>Victoires</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -5080,7 +4429,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nombre de défaites</t>
+          <t>Défaites</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -5102,7 +4451,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Durée moyenne des parties</t>
+          <t>Durée moyenne</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -5114,7 +4463,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Partie la plus rapide</t>
+          <t>Plus court</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -5126,7 +4475,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Partie la plus longue</t>
+          <t>Plus long</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -5136,9 +4485,9 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Statistiques par joueur</t>
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Statistiques des joueurs</t>
         </is>
       </c>
     </row>
@@ -5155,32 +4504,32 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Kills moy.</t>
+          <t>Kills/G</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>Deaths moy.</t>
+          <t>Deaths/G</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Assists moy.</t>
+          <t>Assists/G</t>
         </is>
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>CS/M moy.</t>
+          <t>CS/min</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Vision moy.</t>
+          <t>Vision/G</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>Champions joués</t>
+          <t>Champions</t>
         </is>
       </c>
     </row>
@@ -5304,68 +4653,9 @@
         </is>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>Détail des parties</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="inlineStr">
-        <is>
-          <t>Match ID</t>
-        </is>
-      </c>
-      <c r="B21" s="2" t="inlineStr">
-        <is>
-          <t>Joueur</t>
-        </is>
-      </c>
-      <c r="C21" s="2" t="inlineStr">
-        <is>
-          <t>Champion</t>
-        </is>
-      </c>
-      <c r="D21" s="2" t="inlineStr">
-        <is>
-          <t>KDA</t>
-        </is>
-      </c>
-      <c r="E21" s="2" t="inlineStr">
-        <is>
-          <t>K/D/A</t>
-        </is>
-      </c>
-      <c r="F21" s="2" t="inlineStr">
-        <is>
-          <t>CS</t>
-        </is>
-      </c>
-      <c r="G21" s="2" t="inlineStr">
-        <is>
-          <t>CS/min</t>
-        </is>
-      </c>
-      <c r="H21" s="2" t="inlineStr">
-        <is>
-          <t>Vision Score</t>
-        </is>
-      </c>
-      <c r="I21" s="2" t="inlineStr">
-        <is>
-          <t>Résultat</t>
-        </is>
-      </c>
-      <c r="J21" s="2" t="inlineStr">
-        <is>
-          <t>Durée</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5377,7 +4667,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5385,29 +4675,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="40" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Statistiques globales de l'équipe KCDQ</t>
+          <t>Statistiques de KCDQ</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nombre de parties jouées</t>
+          <t>Matchs joués</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -5417,7 +4705,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nombre de victoires</t>
+          <t>Victoires</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -5427,7 +4715,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nombre de défaites</t>
+          <t>Défaites</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -5449,7 +4737,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Durée moyenne des parties</t>
+          <t>Durée moyenne</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -5461,7 +4749,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Partie la plus rapide</t>
+          <t>Plus court</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -5473,7 +4761,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Partie la plus longue</t>
+          <t>Plus long</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -5483,9 +4771,9 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Statistiques par joueur</t>
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Statistiques des joueurs</t>
         </is>
       </c>
     </row>
@@ -5502,32 +4790,32 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Kills moy.</t>
+          <t>Kills/G</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>Deaths moy.</t>
+          <t>Deaths/G</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Assists moy.</t>
+          <t>Assists/G</t>
         </is>
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>CS/M moy.</t>
+          <t>CS/min</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Vision moy.</t>
+          <t>Vision/G</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>Champions joués</t>
+          <t>Champions</t>
         </is>
       </c>
     </row>
@@ -5681,68 +4969,9 @@
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Détail des parties</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>Match ID</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>Joueur</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>Champion</t>
-        </is>
-      </c>
-      <c r="D22" s="2" t="inlineStr">
-        <is>
-          <t>KDA</t>
-        </is>
-      </c>
-      <c r="E22" s="2" t="inlineStr">
-        <is>
-          <t>K/D/A</t>
-        </is>
-      </c>
-      <c r="F22" s="2" t="inlineStr">
-        <is>
-          <t>CS</t>
-        </is>
-      </c>
-      <c r="G22" s="2" t="inlineStr">
-        <is>
-          <t>CS/min</t>
-        </is>
-      </c>
-      <c r="H22" s="2" t="inlineStr">
-        <is>
-          <t>Vision Score</t>
-        </is>
-      </c>
-      <c r="I22" s="2" t="inlineStr">
-        <is>
-          <t>Résultat</t>
-        </is>
-      </c>
-      <c r="J22" s="2" t="inlineStr">
-        <is>
-          <t>Durée</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5754,7 +4983,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5762,29 +4991,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="40" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Statistiques globales de l'équipe La bande du PMU</t>
+          <t>Statistiques de La bande du PMU</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nombre de parties jouées</t>
+          <t>Matchs joués</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -5794,7 +5021,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nombre de victoires</t>
+          <t>Victoires</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -5804,7 +5031,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nombre de défaites</t>
+          <t>Défaites</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -5826,7 +5053,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Durée moyenne des parties</t>
+          <t>Durée moyenne</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -5838,7 +5065,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Partie la plus rapide</t>
+          <t>Plus court</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -5850,7 +5077,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Partie la plus longue</t>
+          <t>Plus long</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -5860,9 +5087,9 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Statistiques par joueur</t>
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Statistiques des joueurs</t>
         </is>
       </c>
     </row>
@@ -5879,32 +5106,32 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Kills moy.</t>
+          <t>Kills/G</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>Deaths moy.</t>
+          <t>Deaths/G</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Assists moy.</t>
+          <t>Assists/G</t>
         </is>
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>CS/M moy.</t>
+          <t>CS/min</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Vision moy.</t>
+          <t>Vision/G</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>Champions joués</t>
+          <t>Champions</t>
         </is>
       </c>
     </row>
@@ -6058,68 +5285,9 @@
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Détail des parties</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>Match ID</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>Joueur</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>Champion</t>
-        </is>
-      </c>
-      <c r="D22" s="2" t="inlineStr">
-        <is>
-          <t>KDA</t>
-        </is>
-      </c>
-      <c r="E22" s="2" t="inlineStr">
-        <is>
-          <t>K/D/A</t>
-        </is>
-      </c>
-      <c r="F22" s="2" t="inlineStr">
-        <is>
-          <t>CS</t>
-        </is>
-      </c>
-      <c r="G22" s="2" t="inlineStr">
-        <is>
-          <t>CS/min</t>
-        </is>
-      </c>
-      <c r="H22" s="2" t="inlineStr">
-        <is>
-          <t>Vision Score</t>
-        </is>
-      </c>
-      <c r="I22" s="2" t="inlineStr">
-        <is>
-          <t>Résultat</t>
-        </is>
-      </c>
-      <c r="J22" s="2" t="inlineStr">
-        <is>
-          <t>Durée</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -6131,7 +5299,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6139,29 +5307,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="40" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Statistiques globales de l'équipe La Ruche</t>
+          <t>Statistiques de La Ruche</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nombre de parties jouées</t>
+          <t>Matchs joués</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -6171,7 +5337,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nombre de victoires</t>
+          <t>Victoires</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -6181,7 +5347,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nombre de défaites</t>
+          <t>Défaites</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -6203,7 +5369,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Durée moyenne des parties</t>
+          <t>Durée moyenne</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -6215,7 +5381,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Partie la plus rapide</t>
+          <t>Plus court</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -6227,7 +5393,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Partie la plus longue</t>
+          <t>Plus long</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -6237,9 +5403,9 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Statistiques par joueur</t>
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Statistiques des joueurs</t>
         </is>
       </c>
     </row>
@@ -6256,32 +5422,32 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Kills moy.</t>
+          <t>Kills/G</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>Deaths moy.</t>
+          <t>Deaths/G</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Assists moy.</t>
+          <t>Assists/G</t>
         </is>
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>CS/M moy.</t>
+          <t>CS/min</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Vision moy.</t>
+          <t>Vision/G</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>Champions joués</t>
+          <t>Champions</t>
         </is>
       </c>
     </row>
@@ -6435,68 +5601,9 @@
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Détail des parties</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>Match ID</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>Joueur</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>Champion</t>
-        </is>
-      </c>
-      <c r="D22" s="2" t="inlineStr">
-        <is>
-          <t>KDA</t>
-        </is>
-      </c>
-      <c r="E22" s="2" t="inlineStr">
-        <is>
-          <t>K/D/A</t>
-        </is>
-      </c>
-      <c r="F22" s="2" t="inlineStr">
-        <is>
-          <t>CS</t>
-        </is>
-      </c>
-      <c r="G22" s="2" t="inlineStr">
-        <is>
-          <t>CS/min</t>
-        </is>
-      </c>
-      <c r="H22" s="2" t="inlineStr">
-        <is>
-          <t>Vision Score</t>
-        </is>
-      </c>
-      <c r="I22" s="2" t="inlineStr">
-        <is>
-          <t>Résultat</t>
-        </is>
-      </c>
-      <c r="J22" s="2" t="inlineStr">
-        <is>
-          <t>Durée</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>